<commit_message>
planning and assignment updated
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AF759F-AB1C-4B6D-AED3-DFF40E2DFB8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F07B1F2-7224-40F5-91D5-D7BD1ABF31B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Week 1</t>
   </si>
@@ -108,10 +108,13 @@
     <t>Done</t>
   </si>
   <si>
-    <t>planned to be done that week</t>
-  </si>
-  <si>
-    <t>worked on that week</t>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Worked on that week</t>
+  </si>
+  <si>
+    <t>Planned to be done that week</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +621,9 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -638,7 +643,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3"/>
     </row>

</xml_diff>

<commit_message>
updated planning and added some networking and social hacking
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F07B1F2-7224-40F5-91D5-D7BD1ABF31B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB236EB-F6A0-4526-B2F4-F4010E876440}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Week 1</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Planned to be done that week</t>
+  </si>
+  <si>
+    <t>Wireshark</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +627,9 @@
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>

</xml_diff>

<commit_message>
finished footprinting and started scanning
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB236EB-F6A0-4526-B2F4-F4010E876440}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4756511-1AC0-486B-B4D3-7EED0EF22FA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Week 1</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Wireshark</t>
+  </si>
+  <si>
+    <t>Working on now</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +173,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,15 +192,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -207,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -503,19 +513,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD347AE-463B-441A-9488-3A95F67913F3}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -547,116 +557,122 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
started xss and csrf
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\CS S3\BasicKnowledgeAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FF16B6-5192-4AF0-873D-2855A742396C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE19E03D-C5D8-423F-9662-D7E3E1E0B7AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Week 1</t>
   </si>
@@ -121,13 +121,16 @@
   </si>
   <si>
     <t>linux</t>
+  </si>
+  <si>
+    <t>Dropped for now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,8 +144,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,16 +208,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -217,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -513,19 +531,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD347AE-463B-441A-9488-3A95F67913F3}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -557,122 +576,127 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
XSS and CSRF finished
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE19E03D-C5D8-423F-9662-D7E3E1E0B7AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24736092-3275-4BDC-AF2D-5C75BACCB3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,17 +534,17 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -576,79 +576,79 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -662,37 +662,37 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
start Path Traversal..etc and added more to password cracking
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\CS S3\BasicKnowledgeAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24736092-3275-4BDC-AF2D-5C75BACCB3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CEEFB-2F96-42E2-8983-D902E2F0416D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,17 +534,17 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -576,79 +576,79 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -662,37 +662,37 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Password cracking and path traversal..etc finished
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CEEFB-2F96-42E2-8983-D902E2F0416D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016B230-24A5-4CEE-9F2D-A43DD99916D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,13 +634,13 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
sniffing and spoofing finished
</commit_message>
<xml_diff>
--- a/Basic Knowledge Assignment planning.xlsx
+++ b/Basic Knowledge Assignment planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\CS S3\BasicKnowledgeAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\CS S3\BasicKnowledgeAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB25B22B-7F85-4987-9073-4573021CBDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D3482-984C-4314-A0D6-2029705AA1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
+    <workbookView xWindow="12150" yWindow="840" windowWidth="15735" windowHeight="11505" xr2:uid="{C48FE3CD-4CC0-421D-9FE0-15690AEC83A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Week 1</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>Dropped for now</t>
+  </si>
+  <si>
+    <t>Web application proxies &amp; webbrowser plugins</t>
+  </si>
+  <si>
+    <t>Seclab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,13 +146,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -216,10 +215,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +233,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -533,18 +531,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD347AE-463B-441A-9488-3A95F67913F3}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -576,123 +574,127 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>

</xml_diff>